<commit_message>
Added a whole bunch of code
</commit_message>
<xml_diff>
--- a/2.Data/FieldData.xlsx
+++ b/2.Data/FieldData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/evert_sprockel_wur_nl/Documents/5.Wageningen/7.Thesis/7.DataAnalysis/RScripts/2.Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/evert_sprockel_wur_nl/Documents/5.Wageningen/7.Thesis/7.DataAnalysis/ThesisRAnalysis/2.Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="11_38AE230EADFB0BBDC981F51D93740FD6917D560E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9E46262-A6F8-4AE2-80DA-5DF69C83506C}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="11_38AE230EADFB0BBDC981F51D93740FD6917D560E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6BF7E8B-0F66-4AE2-B584-469E85DA525A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -822,12 +822,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -842,7 +848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -862,6 +868,12 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,9 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T16" sqref="T16"/>
+      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1880,63 +1892,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="14">
         <v>45524</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="14">
         <v>0.54513888889050577</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="15">
         <v>33.3643</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="15">
         <v>78.0137</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="13">
         <v>0.38740849999999999</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="13">
         <v>21.5</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
         <v>94.8</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="13">
         <v>0.10000000000000051</v>
       </c>
-      <c r="O12" s="2">
-        <v>0</v>
-      </c>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="2">
+      <c r="O12" s="13">
+        <v>0</v>
+      </c>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="13">
         <v>2</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="R12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="S12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="U12" s="2">
-        <v>0</v>
-      </c>
-      <c r="V12" s="2">
-        <v>0</v>
-      </c>
-      <c r="W12" s="2" t="s">
+      <c r="U12" s="13">
+        <v>0</v>
+      </c>
+      <c r="V12" s="13">
+        <v>0</v>
+      </c>
+      <c r="W12" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4853,74 +4865,74 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="14">
         <v>45534</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="14">
         <v>0.52083333333212067</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="15">
         <v>33.324021000000002</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="15">
         <v>78.038394999999994</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="13">
         <v>0.4169447</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="13">
         <v>19.7</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="13">
         <v>15</v>
       </c>
-      <c r="J55" s="2">
+      <c r="J55" s="13">
         <v>67.5</v>
       </c>
-      <c r="K55" s="2">
+      <c r="K55" s="13">
         <v>7.75</v>
       </c>
-      <c r="L55" s="2">
+      <c r="L55" s="13">
         <v>610.79999999999995</v>
       </c>
-      <c r="M55" s="2">
+      <c r="M55" s="13">
         <v>8429.0399999999991</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N55" s="13">
         <v>7.6000000000000014</v>
       </c>
-      <c r="O55" s="2">
+      <c r="O55" s="13">
         <v>6.9</v>
       </c>
-      <c r="P55" s="12">
+      <c r="P55" s="16">
         <v>0.37</v>
       </c>
-      <c r="Q55" s="2">
+      <c r="Q55" s="13">
         <v>5</v>
       </c>
-      <c r="R55" s="2" t="s">
+      <c r="R55" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="S55" s="2" t="s">
+      <c r="S55" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="T55" s="2" t="s">
+      <c r="T55" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U55" s="2">
+      <c r="U55" s="13">
         <v>1</v>
       </c>
-      <c r="V55" s="2">
-        <v>0</v>
-      </c>
-      <c r="W55" s="2" t="s">
+      <c r="V55" s="13">
+        <v>0</v>
+      </c>
+      <c r="W55" s="13" t="s">
         <v>139</v>
       </c>
     </row>
@@ -7131,71 +7143,71 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="88" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="14">
         <v>45536</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="14">
         <v>0.42361111110949418</v>
       </c>
-      <c r="D88" s="5">
+      <c r="D88" s="15">
         <v>33.256832000000003</v>
       </c>
-      <c r="E88" s="5">
+      <c r="E88" s="15">
         <v>78.049839000000006</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G88" s="2">
+      <c r="G88" s="13">
         <v>0.34255839999999999</v>
       </c>
-      <c r="H88" s="2">
+      <c r="H88" s="13">
         <v>14.4</v>
       </c>
-      <c r="I88" s="2">
+      <c r="I88" s="13">
         <v>77</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J88" s="13">
         <v>56.27</v>
       </c>
-      <c r="K88" s="2">
+      <c r="K88" s="13">
         <v>9.1</v>
       </c>
-      <c r="L88" s="2">
+      <c r="L88" s="13">
         <v>5010</v>
       </c>
-      <c r="M88" s="2">
+      <c r="M88" s="13">
         <v>47595</v>
       </c>
-      <c r="N88" s="2">
+      <c r="N88" s="13">
         <v>0.20000000000000021</v>
       </c>
-      <c r="O88" s="2">
+      <c r="O88" s="13">
         <v>6.5</v>
       </c>
-      <c r="P88" s="12">
+      <c r="P88" s="16">
         <v>1.083</v>
       </c>
-      <c r="Q88" s="2">
+      <c r="Q88" s="13">
         <v>6</v>
       </c>
-      <c r="R88" s="2" t="s">
+      <c r="R88" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="S88" s="2" t="s">
+      <c r="S88" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T88" s="2" t="s">
+      <c r="T88" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="U88" s="2">
-        <v>0</v>
-      </c>
-      <c r="V88" s="2">
+      <c r="U88" s="13">
+        <v>0</v>
+      </c>
+      <c r="V88" s="13">
         <v>0</v>
       </c>
     </row>

</xml_diff>